<commit_message>
fix sd.html search include.
</commit_message>
<xml_diff>
--- a/docs/template-basic2.xlsx
+++ b/docs/template-basic2.xlsx
@@ -9,13 +9,13 @@
     <sheet name="Elements" r:id="rId3" sheetId="1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AK$28</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AL$28</definedName>
   </definedNames>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="927" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="955" uniqueCount="214">
   <si>
     <t>Path</t>
   </si>
@@ -126,6 +126,9 @@
   </si>
   <si>
     <t>Mapping: W5 Mapping</t>
+  </si>
+  <si>
+    <t>Mapping: FiveWs Pattern</t>
   </si>
   <si>
     <t>Basic</t>
@@ -151,13 +154,10 @@
   </si>
   <si>
     <t>dom-2:If the resource is contained in another resource, it SHALL NOT contain nested Resources {contained.contained.empty()}
-dom-1:If the resource is contained in another resource, it SHALL NOT contain any narrative {contained.text.empty()}dom-4:If a resource is contained in another resource, it SHALL NOT have a meta.versionId or a meta.lastUpdated {contained.meta.versionId.empty() and contained.meta.lastUpdated.empty()}dom-3:If the resource is contained in another resource, it SHALL be referred to from elsewhere in the resource {contained.where(('#'+id in %resource.descendants().reference).not()).empty()}temp-1:Identifier SHALL be greater than 5 characters {Identifier.value.length()&gt;5}</t>
+dom-1:If the resource is contained in another resource, it SHALL NOT contain any narrative {contained.text.empty()}dom-4:If a resource is contained in another resource, it SHALL NOT have a meta.versionId or a meta.lastUpdated {contained.meta.versionId.empty() and contained.meta.lastUpdated.empty()}dom-3:If the resource is contained in another resource, it SHALL be referred to from elsewhere in the resource or SHALL refer to the containing resource {contained.all(('#'+id in (%resource.descendants().reference | %resource.descendants().as(canonical))) or descendants().where(reference = '#').exists() or descendants().where(as(canonical) = '#').exists())}temp-1:Identifier SHALL be greater than 5 characters {Identifier.value.length()&gt;5}</t>
   </si>
   <si>
     <t>Act, Entity or Role</t>
-  </si>
-  <si>
-    <t>infrastructure.structure</t>
   </si>
   <si>
     <t>Basic.id</t>
@@ -195,7 +195,7 @@
     <t>Metadata about the resource</t>
   </si>
   <si>
-    <t>The metadata about the resource. This is content that is maintained by the infrastructure. Changes to the content may not always be associated with version changes to the resource.</t>
+    <t>The metadata about the resource. This is content that is maintained by the infrastructure. Changes to the content might not always be associated with version changes to the resource.</t>
   </si>
   <si>
     <t>Resource.meta</t>
@@ -211,11 +211,10 @@
     <t>A set of rules under which this content was created</t>
   </si>
   <si>
-    <t>A reference to a set of rules that were followed when the resource was constructed, and which must be understood when processing the content.</t>
-  </si>
-  <si>
-    <t>Asserting this rule set restricts the content to be only understood by a limited set of trading partners. This inherently limits the usefulness of the data in the long term. However, the existing health eco-system is highly fractured, and not yet ready to define, collect, and exchange data in a generally computable sense. Wherever possible, implementers and/or specification writers should avoid using this element. 
-This element is labelled as a modifier because the implicit rules may provide additional knowledge about the resource that modifies it's meaning or interpretation.</t>
+    <t>A reference to a set of rules that were followed when the resource was constructed, and which must be understood when processing the content. Often, this is a reference to an implementation guide that defines the special rules along with other profiles etc.</t>
+  </si>
+  <si>
+    <t>Asserting this rule set restricts the content to be only understood by a limited set of trading partners. This inherently limits the usefulness of the data in the long term. However, the existing health eco-system is highly fractured, and not yet ready to define, collect, and exchange data in a generally computable sense. Wherever possible, implementers and/or specification writers should avoid using this element. Often, when used, the URL is a reference to an implementation guide that defines these special rules as part of it's narrative along with other profiles, value sets, etc.</t>
   </si>
   <si>
     <t>Resource.implicitRules</t>
@@ -234,7 +233,7 @@
     <t>The base language in which the resource is written.</t>
   </si>
   <si>
-    <t>Language is provided to support indexing and accessibility (typically, services such as text to speech use the language tag). The html language tag in the narrative applies  to the narrative. The language tag on the resource may be used to specify the language of other presentations generated from the data in the resource  Not all the content has to be in the base language. The Resource.language should not be assumed to apply to the narrative automatically. If a language is specified, it should it also be specified on the div element in the html (see rules in HTML5 for information about the relationship between xml:lang and the html lang attribute).</t>
+    <t>Language is provided to support indexing and accessibility (typically, services such as text to speech use the language tag). The html language tag in the narrative applies  to the narrative. The language tag on the resource may be used to specify the language of other presentations generated from the data in the resource. Not all the content has to be in the base language. The Resource.language should not be assumed to apply to the narrative automatically. If a language is specified, it should it also be specified on the div element in the html (see rules in HTML5 for information about the relationship between xml:lang and the html lang attribute).</t>
   </si>
   <si>
     <t>extensible</t>
@@ -263,7 +262,7 @@
     <t>Text summary of the resource, for human interpretation</t>
   </si>
   <si>
-    <t>A human-readable narrative that contains a summary of the resource, and may be used to represent the content of the resource to a human. The narrative need not encode all the structured data, but is required to contain sufficient detail to make it "clinically safe" for a human to just read the narrative. Resource definitions may define what content should be represented in the narrative to ensure clinical safety.</t>
+    <t>A human-readable narrative that contains a summary of the resource and can be used to represent the content of the resource to a human. The narrative need not encode all the structured data, but is required to contain sufficient detail to make it "clinically safe" for a human to just read the narrative. Resource definitions may define what content should be represented in the narrative to ensure clinical safety.</t>
   </si>
   <si>
     <t>Contained resources do not have narrative. Resources that are not contained SHOULD have a narrative. In some cases, a resource may only have text with little or no additional discrete data (as long as all minOccurs=1 elements are satisfied).  This may be necessary for data from legacy systems where information is captured as a "text blob" or where text is additionally entered raw or narrated and encoded in formation is added later.</t>
@@ -364,7 +363,7 @@
     <t>Extensions that cannot be ignored</t>
   </si>
   <si>
-    <t>May be used to represent additional information that is not part of the basic definition of the resource, and that modifies the understanding of the element that contains it. Usually modifier elements provide negation or qualification. In order to make the use of extensions safe and manageable, there is a strict set of governance applied to the definition and use of extensions. Though any implementer is allowed to define an extension, there is a set of requirements that SHALL be met as part of the definition of the extension. Applications processing a resource are required to check for modifier extensions.</t>
+    <t>May be used to represent additional information that is not part of the basic definition of the resource, and that modifies the understanding of the element that contains it. Usually modifier elements provide negation or qualification. To make the use of extensions safe and manageable, there is a strict set of governance applied to the definition and use of extensions. Though any implementer is allowed to define an extension, there is a set of requirements that SHALL be met as part of the definition of the extension. Applications processing a resource are required to check for modifier extensions.</t>
   </si>
   <si>
     <t>There can be no stigma associated with the use of extensions by any application, project, or standard - regardless of the institution or jurisdiction that uses or defines the extensions.  The use of extensions is what allows the FHIR specification to retain a core level of simplicity for everyone.</t>
@@ -395,7 +394,7 @@
     <t>./identifier</t>
   </si>
   <si>
-    <t>id</t>
+    <t>FiveWs.identifier</t>
   </si>
   <si>
     <t>Basic.code</t>
@@ -412,7 +411,7 @@
   </si>
   <si>
     <t>Because resource references will only be able to indicate 'Basic', the type of reference will need to be specified in a Profile identified as part of the resource.  Refer to the resource notes section for information on appropriate terminologies for this code.
-This element is labeled as a modifier because the it defines the meaning of the resource and cannot be ignored.</t>
+This element is labeled as a modifier because it defines the meaning of the resource and cannot be ignored.</t>
   </si>
   <si>
     <t>Must be able to distinguish different types of Basic resources.</t>
@@ -430,7 +429,7 @@
     <t>./code</t>
   </si>
   <si>
-    <t>what</t>
+    <t>FiveWs.what[x]</t>
   </si>
   <si>
     <t>Basic.code.id</t>
@@ -443,7 +442,7 @@
     <t>xml:id (or equivalent in JSON)</t>
   </si>
   <si>
-    <t>unique id for the element within a resource (for internal references). This may be any string value that does not contain spaces.</t>
+    <t>Unique id for the element within a resource (for internal references). This may be any string value that does not contain spaces.</t>
   </si>
   <si>
     <t>Element.id</t>
@@ -455,10 +454,10 @@
     <t>Basic.code.extension</t>
   </si>
   <si>
-    <t>Additional Content defined by implementations</t>
-  </si>
-  <si>
-    <t>May be used to represent additional information that is not part of the basic definition of the element. In order to make the use of extensions safe and manageable, there is a strict set of governance  applied to the definition and use of extensions. Though any implementer is allowed to define an extension, there is a set of requirements that SHALL be met as part of the definition of the extension.</t>
+    <t>Additional content defined by implementations</t>
+  </si>
+  <si>
+    <t>May be used to represent additional information that is not part of the basic definition of the element. To make the use of extensions safe and manageable, there is a strict set of governance  applied to the definition and use of extensions. Though any implementer can define an extension, there is a set of requirements that SHALL be met as part of the definition of the extension.</t>
   </si>
   <si>
     <t>Extensions are always sliced by (at least) url</t>
@@ -507,7 +506,7 @@
     <t>The identification of the code system that defines the meaning of the symbol in the code.</t>
   </si>
   <si>
-    <t>The URI may be an OID (urn:oid:...) or a UUID (urn:uuid:...).  OIDs and UUIDs SHALL be references to the HL7 OID registry. Otherwise, the URI should come from HL7's list of FHIR defined special URIs or it should de-reference to some definition that establish the system clearly and unambiguously.</t>
+    <t>The URI may be an OID (urn:oid:...) or a UUID (urn:uuid:...).  OIDs and UUIDs SHALL be references to the HL7 OID registry. Otherwise, the URI should come from HL7's list of FHIR defined special URIs or it should reference to some definition that establishes the system clearly and unambiguously.</t>
   </si>
   <si>
     <t>Need to be unambiguous about the source of the definition of the symbol.</t>
@@ -525,7 +524,7 @@
     <t>Version of the system - if relevant</t>
   </si>
   <si>
-    <t>The version of the code system which was used when choosing this code. Note that a well-maintained code system does not need the version reported, because the meaning of codes is consistent across versions. However this cannot consistently be assured. and when the meaning is not guaranteed to be consistent, the version SHOULD be exchanged.</t>
+    <t>The version of the code system which was used when choosing this code. Note that a well-maintained code system does not need the version reported, because the meaning of codes is consistent across versions. However this cannot consistently be assured, and when the meaning is not guaranteed to be consistent, the version SHOULD be exchanged.</t>
   </si>
   <si>
     <t>Where the terminology does not clearly define what string should be used to identify code system versions, the recommendation is to use the date (expressed in FHIR date format) on which that version was officially published as the version date.</t>
@@ -641,7 +640,7 @@
     <t>./participation[typeCode='SBJ'] (possibly through a ControlAct and Role)</t>
   </si>
   <si>
-    <t>who.focus</t>
+    <t>FiveWs.subject</t>
   </si>
   <si>
     <t>Basic.created</t>
@@ -663,7 +662,7 @@
     <t>./participation[typeCode='AUT']/time (possibly through a ControlAct and Role)</t>
   </si>
   <si>
-    <t>when.recorded</t>
+    <t>FiveWs.recorded</t>
   </si>
   <si>
     <t>Basic.author</t>
@@ -685,7 +684,7 @@
     <t>./participation[typeCode='SUB'] (possibly through a ControlAct and Role)</t>
   </si>
   <si>
-    <t>who.author</t>
+    <t>FiveWs.author</t>
   </si>
 </sst>
 </file>
@@ -834,7 +833,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AL28"/>
+  <dimension ref="A1:AM28"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -879,7 +878,8 @@
     <col min="34" max="34" width="12.71875" customWidth="true" bestFit="true"/>
     <col min="35" max="35" width="100.703125" customWidth="true"/>
     <col min="36" max="36" width="75.62109375" customWidth="true" bestFit="true"/>
-    <col min="37" max="37" width="23.26171875" customWidth="true" bestFit="true"/>
+    <col min="37" max="37" width="22.0078125" customWidth="true" bestFit="true"/>
+    <col min="38" max="38" width="24.26171875" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -994,108 +994,114 @@
       <c r="AK1" t="s" s="1">
         <v>36</v>
       </c>
+      <c r="AL1" t="s" s="1">
+        <v>37</v>
+      </c>
     </row>
     <row r="2" hidden="true">
       <c r="A2" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" t="s" s="2">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" t="s" s="2">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F2" t="s" s="2">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G2" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H2" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="I2" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="J2" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="K2" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="L2" t="s" s="2">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
       <c r="O2" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="P2" s="2"/>
       <c r="Q2" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="R2" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="S2" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="T2" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="U2" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="V2" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="W2" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="X2" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="Y2" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="Z2" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AA2" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AB2" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AC2" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AD2" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AE2" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AF2" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AG2" t="s" s="2">
         <v>41</v>
       </c>
-      <c r="R2" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="S2" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="T2" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="U2" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="V2" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="W2" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="X2" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="Y2" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="Z2" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AA2" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AB2" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AC2" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AD2" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AE2" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AF2" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AG2" t="s" s="2">
-        <v>40</v>
-      </c>
       <c r="AH2" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AI2" t="s" s="2">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="AJ2" t="s" s="2">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="AK2" t="s" s="2">
-        <v>46</v>
+        <v>42</v>
+      </c>
+      <c r="AL2" t="s" s="2">
+        <v>42</v>
       </c>
     </row>
     <row r="3" hidden="true">
@@ -1104,20 +1110,20 @@
       </c>
       <c r="B3" s="2"/>
       <c r="C3" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" t="s" s="2">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F3" t="s" s="2">
         <v>48</v>
       </c>
       <c r="G3" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H3" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="I3" t="s" s="2">
         <v>49</v>
@@ -1136,71 +1142,74 @@
       </c>
       <c r="N3" s="2"/>
       <c r="O3" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="P3" s="2"/>
       <c r="Q3" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="R3" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="S3" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="T3" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="U3" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="V3" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="W3" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="X3" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="Y3" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="Z3" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AA3" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AB3" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AC3" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AD3" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AE3" t="s" s="2">
         <v>54</v>
       </c>
       <c r="AF3" t="s" s="2">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="AG3" t="s" s="2">
         <v>48</v>
       </c>
       <c r="AH3" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AI3" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AJ3" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AK3" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
+      </c>
+      <c r="AL3" t="s" s="2">
+        <v>42</v>
       </c>
     </row>
     <row r="4" hidden="true">
@@ -1209,20 +1218,20 @@
       </c>
       <c r="B4" s="2"/>
       <c r="C4" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" t="s" s="2">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F4" t="s" s="2">
         <v>48</v>
       </c>
       <c r="G4" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H4" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="I4" t="s" s="2">
         <v>49</v>
@@ -1239,71 +1248,74 @@
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
       <c r="O4" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="P4" s="2"/>
       <c r="Q4" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="R4" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="S4" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="T4" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="U4" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="V4" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="W4" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="X4" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="Y4" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="Z4" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AA4" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AB4" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AC4" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AD4" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AE4" t="s" s="2">
         <v>59</v>
       </c>
       <c r="AF4" t="s" s="2">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="AG4" t="s" s="2">
         <v>48</v>
       </c>
       <c r="AH4" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AI4" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AJ4" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AK4" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
+      </c>
+      <c r="AL4" t="s" s="2">
+        <v>42</v>
       </c>
     </row>
     <row r="5" hidden="true">
@@ -1312,17 +1324,17 @@
       </c>
       <c r="B5" s="2"/>
       <c r="C5" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" t="s" s="2">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F5" t="s" s="2">
         <v>48</v>
       </c>
       <c r="G5" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H5" t="s" s="2">
         <v>49</v>
@@ -1344,71 +1356,74 @@
       </c>
       <c r="N5" s="2"/>
       <c r="O5" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="P5" s="2"/>
       <c r="Q5" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="R5" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="S5" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="T5" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="U5" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="V5" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="W5" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="X5" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="Y5" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="Z5" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AA5" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AB5" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AC5" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AD5" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AE5" t="s" s="2">
         <v>65</v>
       </c>
       <c r="AF5" t="s" s="2">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="AG5" t="s" s="2">
         <v>48</v>
       </c>
       <c r="AH5" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AI5" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AJ5" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AK5" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
+      </c>
+      <c r="AL5" t="s" s="2">
+        <v>42</v>
       </c>
     </row>
     <row r="6" hidden="true">
@@ -1417,23 +1432,23 @@
       </c>
       <c r="B6" s="2"/>
       <c r="C6" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" t="s" s="2">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F6" t="s" s="2">
         <v>48</v>
       </c>
       <c r="G6" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H6" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="I6" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="J6" t="s" s="2">
         <v>67</v>
@@ -1449,26 +1464,26 @@
       </c>
       <c r="N6" s="2"/>
       <c r="O6" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="P6" s="2"/>
       <c r="Q6" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="R6" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="S6" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="T6" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="U6" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="V6" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="W6" t="s" s="2">
         <v>71</v>
@@ -1480,40 +1495,43 @@
         <v>73</v>
       </c>
       <c r="Z6" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AA6" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AB6" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AC6" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AD6" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AE6" t="s" s="2">
         <v>74</v>
       </c>
       <c r="AF6" t="s" s="2">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="AG6" t="s" s="2">
         <v>48</v>
       </c>
       <c r="AH6" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AI6" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AJ6" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AK6" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
+      </c>
+      <c r="AL6" t="s" s="2">
+        <v>42</v>
       </c>
     </row>
     <row r="7" hidden="true">
@@ -1526,19 +1544,19 @@
       </c>
       <c r="D7" s="2"/>
       <c r="E7" t="s" s="2">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F7" t="s" s="2">
         <v>48</v>
       </c>
       <c r="G7" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H7" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="I7" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="J7" t="s" s="2">
         <v>77</v>
@@ -1554,56 +1572,56 @@
       </c>
       <c r="N7" s="2"/>
       <c r="O7" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="P7" s="2"/>
       <c r="Q7" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="R7" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="S7" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="T7" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="U7" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="V7" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="W7" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="X7" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="Y7" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="Z7" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AA7" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AB7" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AC7" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AD7" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AE7" t="s" s="2">
         <v>81</v>
       </c>
       <c r="AF7" t="s" s="2">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="AG7" t="s" s="2">
         <v>48</v>
@@ -1612,13 +1630,16 @@
         <v>82</v>
       </c>
       <c r="AI7" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AJ7" t="s" s="2">
         <v>83</v>
       </c>
       <c r="AK7" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
+      </c>
+      <c r="AL7" t="s" s="2">
+        <v>42</v>
       </c>
     </row>
     <row r="8" hidden="true">
@@ -1631,19 +1652,19 @@
       </c>
       <c r="D8" s="2"/>
       <c r="E8" t="s" s="2">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F8" t="s" s="2">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G8" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H8" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="I8" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="J8" t="s" s="2">
         <v>86</v>
@@ -1659,71 +1680,74 @@
       </c>
       <c r="N8" s="2"/>
       <c r="O8" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="P8" s="2"/>
       <c r="Q8" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="R8" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="S8" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="T8" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="U8" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="V8" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="W8" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="X8" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="Y8" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="Z8" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AA8" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AB8" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AC8" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AD8" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AE8" t="s" s="2">
         <v>90</v>
       </c>
       <c r="AF8" t="s" s="2">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="AG8" t="s" s="2">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="AH8" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AI8" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AJ8" t="s" s="2">
         <v>91</v>
       </c>
       <c r="AK8" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
+      </c>
+      <c r="AL8" t="s" s="2">
+        <v>42</v>
       </c>
     </row>
     <row r="9" hidden="true">
@@ -1732,23 +1756,23 @@
       </c>
       <c r="B9" s="2"/>
       <c r="C9" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" t="s" s="2">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F9" t="s" s="2">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G9" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H9" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="I9" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="J9" t="s" s="2">
         <v>93</v>
@@ -1762,45 +1786,45 @@
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>
       <c r="O9" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="P9" s="2"/>
       <c r="Q9" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="R9" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="S9" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="T9" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="U9" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="V9" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="W9" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="X9" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="Y9" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="Z9" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AA9" t="s" s="2">
         <v>96</v>
       </c>
       <c r="AB9" s="2"/>
       <c r="AC9" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AD9" t="s" s="2">
         <v>97</v>
@@ -1809,22 +1833,25 @@
         <v>98</v>
       </c>
       <c r="AF9" t="s" s="2">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="AG9" t="s" s="2">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="AH9" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AI9" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AJ9" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AK9" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
+      </c>
+      <c r="AL9" t="s" s="2">
+        <v>42</v>
       </c>
     </row>
     <row r="10">
@@ -1835,11 +1862,11 @@
         <v>99</v>
       </c>
       <c r="C10" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" t="s" s="2">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F10" t="s" s="2">
         <v>48</v>
@@ -1848,10 +1875,10 @@
         <v>49</v>
       </c>
       <c r="H10" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="I10" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="J10" t="s" s="2">
         <v>100</v>
@@ -1865,71 +1892,74 @@
       <c r="M10" s="2"/>
       <c r="N10" s="2"/>
       <c r="O10" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="P10" s="2"/>
       <c r="Q10" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="R10" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="S10" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="T10" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="U10" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="V10" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="W10" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="X10" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="Y10" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="Z10" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AA10" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AB10" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AC10" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AD10" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AE10" t="s" s="2">
         <v>98</v>
       </c>
       <c r="AF10" t="s" s="2">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="AG10" t="s" s="2">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="AH10" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AI10" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AJ10" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AK10" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
+      </c>
+      <c r="AL10" t="s" s="2">
+        <v>42</v>
       </c>
     </row>
     <row r="11">
@@ -1940,11 +1970,11 @@
         <v>103</v>
       </c>
       <c r="C11" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" t="s" s="2">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F11" t="s" s="2">
         <v>48</v>
@@ -1953,10 +1983,10 @@
         <v>49</v>
       </c>
       <c r="H11" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="I11" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="J11" t="s" s="2">
         <v>104</v>
@@ -1970,71 +2000,74 @@
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
       <c r="O11" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="P11" s="2"/>
       <c r="Q11" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="R11" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="S11" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="T11" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="U11" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="V11" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="W11" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="X11" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="Y11" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="Z11" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AA11" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AB11" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AC11" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AD11" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AE11" t="s" s="2">
         <v>98</v>
       </c>
       <c r="AF11" t="s" s="2">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="AG11" t="s" s="2">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="AH11" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AI11" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AJ11" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AK11" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
+      </c>
+      <c r="AL11" t="s" s="2">
+        <v>42</v>
       </c>
     </row>
     <row r="12" hidden="true">
@@ -2047,19 +2080,19 @@
       </c>
       <c r="D12" s="2"/>
       <c r="E12" t="s" s="2">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F12" t="s" s="2">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G12" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H12" t="s" s="2">
         <v>49</v>
       </c>
       <c r="I12" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="J12" t="s" s="2">
         <v>93</v>
@@ -2075,71 +2108,74 @@
       </c>
       <c r="N12" s="2"/>
       <c r="O12" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="P12" s="2"/>
       <c r="Q12" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="R12" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="S12" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="T12" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="U12" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="V12" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="W12" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="X12" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="Y12" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="Z12" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AA12" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AB12" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AC12" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AD12" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AE12" t="s" s="2">
         <v>112</v>
       </c>
       <c r="AF12" t="s" s="2">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="AG12" t="s" s="2">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="AH12" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AI12" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AJ12" t="s" s="2">
         <v>91</v>
       </c>
       <c r="AK12" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
+      </c>
+      <c r="AL12" t="s" s="2">
+        <v>42</v>
       </c>
     </row>
     <row r="13">
@@ -2148,7 +2184,7 @@
       </c>
       <c r="B13" s="2"/>
       <c r="C13" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" t="s" s="2">
@@ -2161,7 +2197,7 @@
         <v>49</v>
       </c>
       <c r="H13" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="I13" t="s" s="2">
         <v>49</v>
@@ -2178,70 +2214,73 @@
       <c r="M13" s="2"/>
       <c r="N13" s="2"/>
       <c r="O13" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="P13" s="2"/>
       <c r="Q13" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="R13" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="S13" t="s" s="2">
         <v>117</v>
       </c>
       <c r="T13" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="U13" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="V13" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="W13" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="X13" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="Y13" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="Z13" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AA13" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AB13" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AC13" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AD13" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AE13" t="s" s="2">
         <v>113</v>
       </c>
       <c r="AF13" t="s" s="2">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="AG13" t="s" s="2">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="AH13" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AI13" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AJ13" t="s" s="2">
         <v>118</v>
       </c>
       <c r="AK13" t="s" s="2">
+        <v>119</v>
+      </c>
+      <c r="AL13" t="s" s="2">
         <v>119</v>
       </c>
     </row>
@@ -2251,7 +2290,7 @@
       </c>
       <c r="B14" s="2"/>
       <c r="C14" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" t="s" s="2">
@@ -2285,26 +2324,26 @@
         <v>125</v>
       </c>
       <c r="O14" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="P14" s="2"/>
       <c r="Q14" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="R14" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="S14" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="T14" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="U14" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="V14" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="W14" t="s" s="2">
         <v>126</v>
@@ -2316,19 +2355,19 @@
         <v>128</v>
       </c>
       <c r="Z14" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AA14" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AB14" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AC14" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AD14" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AE14" t="s" s="2">
         <v>120</v>
@@ -2340,15 +2379,18 @@
         <v>48</v>
       </c>
       <c r="AH14" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AI14" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AJ14" t="s" s="2">
         <v>129</v>
       </c>
       <c r="AK14" t="s" s="2">
+        <v>130</v>
+      </c>
+      <c r="AL14" t="s" s="2">
         <v>130</v>
       </c>
     </row>
@@ -2358,23 +2400,23 @@
       </c>
       <c r="B15" s="2"/>
       <c r="C15" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D15" s="2"/>
       <c r="E15" t="s" s="2">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F15" t="s" s="2">
         <v>48</v>
       </c>
       <c r="G15" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H15" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="I15" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="J15" t="s" s="2">
         <v>132</v>
@@ -2388,71 +2430,74 @@
       <c r="M15" s="2"/>
       <c r="N15" s="2"/>
       <c r="O15" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="P15" s="2"/>
       <c r="Q15" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="R15" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="S15" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="T15" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="U15" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="V15" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="W15" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="X15" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="Y15" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="Z15" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AA15" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AB15" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AC15" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AD15" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AE15" t="s" s="2">
         <v>135</v>
       </c>
       <c r="AF15" t="s" s="2">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="AG15" t="s" s="2">
         <v>48</v>
       </c>
       <c r="AH15" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AI15" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AJ15" t="s" s="2">
         <v>136</v>
       </c>
       <c r="AK15" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
+      </c>
+      <c r="AL15" t="s" s="2">
+        <v>42</v>
       </c>
     </row>
     <row r="16" hidden="true">
@@ -2465,19 +2510,19 @@
       </c>
       <c r="D16" s="2"/>
       <c r="E16" t="s" s="2">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F16" t="s" s="2">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G16" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H16" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="I16" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="J16" t="s" s="2">
         <v>93</v>
@@ -2493,38 +2538,38 @@
       </c>
       <c r="N16" s="2"/>
       <c r="O16" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="P16" s="2"/>
       <c r="Q16" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="R16" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="S16" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="T16" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="U16" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="V16" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="W16" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="X16" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="Y16" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="Z16" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AA16" t="s" s="2">
         <v>96</v>
@@ -2533,7 +2578,7 @@
         <v>140</v>
       </c>
       <c r="AC16" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AD16" t="s" s="2">
         <v>97</v>
@@ -2542,22 +2587,25 @@
         <v>141</v>
       </c>
       <c r="AF16" t="s" s="2">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="AG16" t="s" s="2">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="AH16" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AI16" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AJ16" t="s" s="2">
         <v>136</v>
       </c>
       <c r="AK16" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
+      </c>
+      <c r="AL16" t="s" s="2">
+        <v>42</v>
       </c>
     </row>
     <row r="17">
@@ -2566,7 +2614,7 @@
       </c>
       <c r="B17" s="2"/>
       <c r="C17" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D17" s="2"/>
       <c r="E17" t="s" s="2">
@@ -2579,7 +2627,7 @@
         <v>49</v>
       </c>
       <c r="H17" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="I17" t="s" s="2">
         <v>49</v>
@@ -2600,71 +2648,74 @@
         <v>147</v>
       </c>
       <c r="O17" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="P17" s="2"/>
       <c r="Q17" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="R17" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="S17" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="T17" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="U17" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="V17" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="W17" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="X17" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="Y17" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="Z17" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AA17" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AB17" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AC17" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AD17" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AE17" t="s" s="2">
         <v>148</v>
       </c>
       <c r="AF17" t="s" s="2">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="AG17" t="s" s="2">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="AH17" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AI17" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AJ17" t="s" s="2">
         <v>149</v>
       </c>
       <c r="AK17" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
+      </c>
+      <c r="AL17" t="s" s="2">
+        <v>42</v>
       </c>
     </row>
     <row r="18" hidden="true">
@@ -2673,23 +2724,23 @@
       </c>
       <c r="B18" s="2"/>
       <c r="C18" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D18" s="2"/>
       <c r="E18" t="s" s="2">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F18" t="s" s="2">
         <v>48</v>
       </c>
       <c r="G18" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H18" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="I18" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="J18" t="s" s="2">
         <v>132</v>
@@ -2703,71 +2754,74 @@
       <c r="M18" s="2"/>
       <c r="N18" s="2"/>
       <c r="O18" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="P18" s="2"/>
       <c r="Q18" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="R18" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="S18" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="T18" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="U18" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="V18" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="W18" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="X18" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="Y18" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="Z18" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AA18" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AB18" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AC18" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AD18" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AE18" t="s" s="2">
         <v>135</v>
       </c>
       <c r="AF18" t="s" s="2">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="AG18" t="s" s="2">
         <v>48</v>
       </c>
       <c r="AH18" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AI18" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AJ18" t="s" s="2">
         <v>136</v>
       </c>
       <c r="AK18" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
+      </c>
+      <c r="AL18" t="s" s="2">
+        <v>42</v>
       </c>
     </row>
     <row r="19" hidden="true">
@@ -2780,19 +2834,19 @@
       </c>
       <c r="D19" s="2"/>
       <c r="E19" t="s" s="2">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F19" t="s" s="2">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G19" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H19" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="I19" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="J19" t="s" s="2">
         <v>93</v>
@@ -2808,38 +2862,38 @@
       </c>
       <c r="N19" s="2"/>
       <c r="O19" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="P19" s="2"/>
       <c r="Q19" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="R19" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="S19" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="T19" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="U19" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="V19" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="W19" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="X19" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="Y19" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="Z19" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AA19" t="s" s="2">
         <v>96</v>
@@ -2848,7 +2902,7 @@
         <v>140</v>
       </c>
       <c r="AC19" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AD19" t="s" s="2">
         <v>97</v>
@@ -2857,22 +2911,25 @@
         <v>141</v>
       </c>
       <c r="AF19" t="s" s="2">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="AG19" t="s" s="2">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="AH19" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AI19" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AJ19" t="s" s="2">
         <v>136</v>
       </c>
       <c r="AK19" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
+      </c>
+      <c r="AL19" t="s" s="2">
+        <v>42</v>
       </c>
     </row>
     <row r="20" hidden="true">
@@ -2881,20 +2938,20 @@
       </c>
       <c r="B20" s="2"/>
       <c r="C20" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D20" s="2"/>
       <c r="E20" t="s" s="2">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F20" t="s" s="2">
         <v>48</v>
       </c>
       <c r="G20" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H20" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="I20" t="s" s="2">
         <v>49</v>
@@ -2915,71 +2972,74 @@
         <v>156</v>
       </c>
       <c r="O20" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="P20" s="2"/>
       <c r="Q20" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="R20" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="S20" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="T20" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="U20" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="V20" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="W20" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="X20" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="Y20" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="Z20" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AA20" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AB20" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AC20" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AD20" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AE20" t="s" s="2">
         <v>157</v>
       </c>
       <c r="AF20" t="s" s="2">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="AG20" t="s" s="2">
         <v>48</v>
       </c>
       <c r="AH20" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AI20" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AJ20" t="s" s="2">
         <v>158</v>
       </c>
       <c r="AK20" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
+      </c>
+      <c r="AL20" t="s" s="2">
+        <v>42</v>
       </c>
     </row>
     <row r="21" hidden="true">
@@ -2988,20 +3048,20 @@
       </c>
       <c r="B21" s="2"/>
       <c r="C21" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D21" s="2"/>
       <c r="E21" t="s" s="2">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F21" t="s" s="2">
         <v>48</v>
       </c>
       <c r="G21" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H21" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="I21" t="s" s="2">
         <v>49</v>
@@ -3020,71 +3080,74 @@
       </c>
       <c r="N21" s="2"/>
       <c r="O21" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="P21" s="2"/>
       <c r="Q21" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="R21" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="S21" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="T21" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="U21" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="V21" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="W21" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="X21" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="Y21" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="Z21" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AA21" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AB21" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AC21" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AD21" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AE21" t="s" s="2">
         <v>163</v>
       </c>
       <c r="AF21" t="s" s="2">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="AG21" t="s" s="2">
         <v>48</v>
       </c>
       <c r="AH21" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AI21" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AJ21" t="s" s="2">
         <v>164</v>
       </c>
       <c r="AK21" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
+      </c>
+      <c r="AL21" t="s" s="2">
+        <v>42</v>
       </c>
     </row>
     <row r="22">
@@ -3093,7 +3156,7 @@
       </c>
       <c r="B22" s="2"/>
       <c r="C22" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D22" s="2"/>
       <c r="E22" t="s" s="2">
@@ -3106,7 +3169,7 @@
         <v>49</v>
       </c>
       <c r="H22" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="I22" t="s" s="2">
         <v>49</v>
@@ -3125,71 +3188,74 @@
         <v>168</v>
       </c>
       <c r="O22" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="P22" s="2"/>
       <c r="Q22" t="s" s="2">
         <v>169</v>
       </c>
       <c r="R22" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="S22" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="T22" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="U22" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="V22" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="W22" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="X22" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="Y22" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="Z22" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AA22" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AB22" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AC22" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AD22" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AE22" t="s" s="2">
         <v>170</v>
       </c>
       <c r="AF22" t="s" s="2">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="AG22" t="s" s="2">
         <v>48</v>
       </c>
       <c r="AH22" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AI22" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AJ22" t="s" s="2">
         <v>129</v>
       </c>
       <c r="AK22" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
+      </c>
+      <c r="AL22" t="s" s="2">
+        <v>42</v>
       </c>
     </row>
     <row r="23" hidden="true">
@@ -3198,20 +3264,20 @@
       </c>
       <c r="B23" s="2"/>
       <c r="C23" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D23" s="2"/>
       <c r="E23" t="s" s="2">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F23" t="s" s="2">
         <v>48</v>
       </c>
       <c r="G23" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H23" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="I23" t="s" s="2">
         <v>49</v>
@@ -3230,71 +3296,74 @@
         <v>174</v>
       </c>
       <c r="O23" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="P23" s="2"/>
       <c r="Q23" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="R23" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="S23" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="T23" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="U23" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="V23" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="W23" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="X23" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="Y23" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="Z23" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AA23" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AB23" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AC23" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AD23" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AE23" t="s" s="2">
         <v>175</v>
       </c>
       <c r="AF23" t="s" s="2">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="AG23" t="s" s="2">
         <v>48</v>
       </c>
       <c r="AH23" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AI23" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AJ23" t="s" s="2">
         <v>176</v>
       </c>
       <c r="AK23" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
+      </c>
+      <c r="AL23" t="s" s="2">
+        <v>42</v>
       </c>
     </row>
     <row r="24" hidden="true">
@@ -3303,20 +3372,20 @@
       </c>
       <c r="B24" s="2"/>
       <c r="C24" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D24" s="2"/>
       <c r="E24" t="s" s="2">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F24" t="s" s="2">
         <v>48</v>
       </c>
       <c r="G24" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H24" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="I24" t="s" s="2">
         <v>49</v>
@@ -3337,71 +3406,74 @@
         <v>182</v>
       </c>
       <c r="O24" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="P24" s="2"/>
       <c r="Q24" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="R24" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="S24" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="T24" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="U24" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="V24" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="W24" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="X24" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="Y24" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="Z24" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AA24" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AB24" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AC24" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AD24" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AE24" t="s" s="2">
         <v>183</v>
       </c>
       <c r="AF24" t="s" s="2">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="AG24" t="s" s="2">
         <v>48</v>
       </c>
       <c r="AH24" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AI24" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AJ24" t="s" s="2">
         <v>184</v>
       </c>
       <c r="AK24" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
+      </c>
+      <c r="AL24" t="s" s="2">
+        <v>42</v>
       </c>
     </row>
     <row r="25" hidden="true">
@@ -3410,20 +3482,20 @@
       </c>
       <c r="B25" s="2"/>
       <c r="C25" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D25" s="2"/>
       <c r="E25" t="s" s="2">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F25" t="s" s="2">
         <v>48</v>
       </c>
       <c r="G25" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H25" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="I25" t="s" s="2">
         <v>49</v>
@@ -3444,71 +3516,74 @@
         <v>189</v>
       </c>
       <c r="O25" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="P25" s="2"/>
       <c r="Q25" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="R25" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="S25" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="T25" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="U25" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="V25" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="W25" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="X25" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="Y25" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="Z25" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AA25" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AB25" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AC25" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AD25" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AE25" t="s" s="2">
         <v>190</v>
       </c>
       <c r="AF25" t="s" s="2">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="AG25" t="s" s="2">
         <v>48</v>
       </c>
       <c r="AH25" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AI25" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AJ25" t="s" s="2">
         <v>191</v>
       </c>
       <c r="AK25" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
+      </c>
+      <c r="AL25" t="s" s="2">
+        <v>42</v>
       </c>
     </row>
     <row r="26">
@@ -3517,7 +3592,7 @@
       </c>
       <c r="B26" s="2"/>
       <c r="C26" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D26" s="2"/>
       <c r="E26" t="s" s="2">
@@ -3530,7 +3605,7 @@
         <v>49</v>
       </c>
       <c r="H26" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="I26" t="s" s="2">
         <v>49</v>
@@ -3551,70 +3626,73 @@
         <v>197</v>
       </c>
       <c r="O26" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="P26" s="2"/>
       <c r="Q26" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="R26" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="S26" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="T26" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="U26" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="V26" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="W26" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="X26" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="Y26" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="Z26" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AA26" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AB26" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AC26" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AD26" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AE26" t="s" s="2">
         <v>192</v>
       </c>
       <c r="AF26" t="s" s="2">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="AG26" t="s" s="2">
         <v>48</v>
       </c>
       <c r="AH26" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AI26" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AJ26" t="s" s="2">
         <v>198</v>
       </c>
       <c r="AK26" t="s" s="2">
+        <v>199</v>
+      </c>
+      <c r="AL26" t="s" s="2">
         <v>199</v>
       </c>
     </row>
@@ -3624,20 +3702,20 @@
       </c>
       <c r="B27" s="2"/>
       <c r="C27" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D27" s="2"/>
       <c r="E27" t="s" s="2">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F27" t="s" s="2">
         <v>48</v>
       </c>
       <c r="G27" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H27" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="I27" t="s" s="2">
         <v>49</v>
@@ -3656,70 +3734,73 @@
         <v>204</v>
       </c>
       <c r="O27" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="P27" s="2"/>
       <c r="Q27" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="R27" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="S27" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="T27" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="U27" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="V27" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="W27" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="X27" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="Y27" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="Z27" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AA27" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AB27" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AC27" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AD27" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AE27" t="s" s="2">
         <v>200</v>
       </c>
       <c r="AF27" t="s" s="2">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="AG27" t="s" s="2">
         <v>48</v>
       </c>
       <c r="AH27" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AI27" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AJ27" t="s" s="2">
         <v>205</v>
       </c>
       <c r="AK27" t="s" s="2">
+        <v>206</v>
+      </c>
+      <c r="AL27" t="s" s="2">
         <v>206</v>
       </c>
     </row>
@@ -3729,20 +3810,20 @@
       </c>
       <c r="B28" s="2"/>
       <c r="C28" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D28" s="2"/>
       <c r="E28" t="s" s="2">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F28" t="s" s="2">
         <v>48</v>
       </c>
       <c r="G28" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H28" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="I28" t="s" s="2">
         <v>49</v>
@@ -3761,65 +3842,65 @@
         <v>211</v>
       </c>
       <c r="O28" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="P28" s="2"/>
       <c r="Q28" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="R28" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="S28" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="T28" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="U28" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="V28" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="W28" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="X28" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="Y28" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="Z28" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AA28" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AB28" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AC28" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AD28" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AE28" t="s" s="2">
         <v>207</v>
       </c>
       <c r="AF28" t="s" s="2">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="AG28" t="s" s="2">
         <v>48</v>
       </c>
       <c r="AH28" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AI28" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AJ28" t="s" s="2">
         <v>212</v>
@@ -3827,9 +3908,12 @@
       <c r="AK28" t="s" s="2">
         <v>213</v>
       </c>
+      <c r="AL28" t="s" s="2">
+        <v>213</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AK28">
+  <autoFilter ref="A1:AL28">
     <filterColumn colId="6">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>

</xml_diff>